<commit_message>
Fixing issue where FeOT values were not considered in calib_plot(). Upgrading also to pip version 0.1.7
</commit_message>
<xml_diff>
--- a/manuscript/Supplement/Datasets/example_data.xlsx
+++ b/manuscript/Supplement/Datasets/example_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kiacovin/Box/Research/__Manuscripts in Progress/__VESIcal/__TheCode/VESIcal/manuscript/Supplement/Example_Datasets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kiacovin/Dropbox/Research/__Manuscripts in Progress/__VESIcal/__TheCode/VESIcal/manuscript/Supplement/Datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A441644-7521-CE43-9DD5-48B2732FC3B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EF45B75-67F9-714D-9D53-CD4CFE86CDB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="6700" windowWidth="33600" windowHeight="20540" xr2:uid="{286DCE04-AB12-484B-880B-42B53AAF1A46}"/>
+    <workbookView xWindow="6420" yWindow="5820" windowWidth="33600" windowHeight="20540" xr2:uid="{286DCE04-AB12-484B-880B-42B53AAF1A46}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -592,7 +592,7 @@
   <dimension ref="A1:U21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T19" sqref="T19"/>
+      <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update pip to v0.9.14
</commit_message>
<xml_diff>
--- a/manuscript/Supplement/Datasets/example_data.xlsx
+++ b/manuscript/Supplement/Datasets/example_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10314"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kiacovin/Dropbox/Research/__Manuscripts in Progress/__VESIcal/__TheCode/VESIcal/manuscript/Supplement/Datasets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kiacovin/Dropbox/Research/__Manuscripts in Progress/__VESIcal/__TheCode/VESIcal_master/VESIcal/manuscript/Supplement/Datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EF45B75-67F9-714D-9D53-CD4CFE86CDB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{949866C3-7FE9-9747-9A08-62CB9EED7DDA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6420" yWindow="5820" windowWidth="33600" windowHeight="20540" xr2:uid="{286DCE04-AB12-484B-880B-42B53AAF1A46}"/>
   </bookViews>
@@ -592,7 +592,7 @@
   <dimension ref="A1:U21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T2" sqref="T2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Upgrade to pip v0.9.15 (my shame in uploading two buggy versions to pip today is forever immortalized on GitHub)
</commit_message>
<xml_diff>
--- a/manuscript/Supplement/Datasets/example_data.xlsx
+++ b/manuscript/Supplement/Datasets/example_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kiacovin/Dropbox/Research/__Manuscripts in Progress/__VESIcal/__TheCode/VESIcal_master/VESIcal/manuscript/Supplement/Datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{949866C3-7FE9-9747-9A08-62CB9EED7DDA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEFCC9A7-6476-9647-9123-3184CDD46C5E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6420" yWindow="5820" windowWidth="33600" windowHeight="20540" xr2:uid="{286DCE04-AB12-484B-880B-42B53AAF1A46}"/>
+    <workbookView xWindow="-260" yWindow="3640" windowWidth="33600" windowHeight="20540" xr2:uid="{286DCE04-AB12-484B-880B-42B53AAF1A46}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -592,7 +592,7 @@
   <dimension ref="A1:U21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>